<commit_message>
raw_hmm, navigation, and heatmap implementation
</commit_message>
<xml_diff>
--- a/CSCG_rooms.xlsx
+++ b/CSCG_rooms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23d5595a8aedaea0/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23d5595a8aedaea0/Desktop/sunLab/CSCG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2E4EA6A-9A94-4578-BDC0-16316EF5C145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{A2E4EA6A-9A94-4578-BDC0-16316EF5C145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B99287F-C894-4970-9C1C-2614568B1FC4}"/>
   <bookViews>
-    <workbookView xWindow="13080" yWindow="0" windowWidth="13337" windowHeight="16543" xr2:uid="{458C665F-2A40-4E60-A8B1-0CDDE2DB9563}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="26537" windowHeight="16663" xr2:uid="{458C665F-2A40-4E60-A8B1-0CDDE2DB9563}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,15 +402,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FCE50A-E014-4B1E-BFB0-7FC930E73456}">
-  <dimension ref="C4:O14"/>
+  <dimension ref="C4:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:O14"/>
+      <selection activeCell="T11" sqref="R9:T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:20" x14ac:dyDescent="0.4">
       <c r="D4">
         <v>0</v>
       </c>
@@ -436,7 +436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:20" x14ac:dyDescent="0.4">
       <c r="D5">
         <v>0</v>
       </c>
@@ -462,7 +462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:20" x14ac:dyDescent="0.4">
       <c r="D6">
         <v>0</v>
       </c>
@@ -488,7 +488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="3:20" x14ac:dyDescent="0.4">
       <c r="D7">
         <v>0</v>
       </c>
@@ -514,7 +514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:20" x14ac:dyDescent="0.4">
       <c r="D8">
         <v>0</v>
       </c>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:20" x14ac:dyDescent="0.4">
       <c r="D9">
         <v>0</v>
       </c>
@@ -565,8 +565,17 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.4">
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>2</v>
+      </c>
+      <c r="T9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.4">
       <c r="D10">
         <v>0</v>
       </c>
@@ -591,8 +600,28 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.4">
+      <c r="R10">
+        <v>4</v>
+      </c>
+      <c r="S10">
+        <v>5</v>
+      </c>
+      <c r="T10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:20" x14ac:dyDescent="0.4">
+      <c r="R11">
+        <v>7</v>
+      </c>
+      <c r="S11">
+        <v>8</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.4">
       <c r="C13">
         <v>0</v>
       </c>
@@ -633,7 +662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="3:20" x14ac:dyDescent="0.4">
       <c r="C14">
         <v>0</v>
       </c>
@@ -672,6 +701,120 @@
       </c>
       <c r="O14">
         <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+      <c r="K26">
+        <v>5</v>
+      </c>
+      <c r="L26">
+        <v>6</v>
+      </c>
+      <c r="M26">
+        <v>7</v>
+      </c>
+      <c r="N26">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>